<commit_message>
Everything done except correction error
The robot goes back pretty much EXACTLY to the right spot, increments X
and Y with to the right values when crossing lines, but still ends up
with a weird offset in the end. I'm going to try and fix this tonight.
</commit_message>
<xml_diff>
--- a/Lab2-Odometry/Report/Lab 2 Report.xlsx
+++ b/Lab2-Odometry/Report/Lab 2 Report.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jlat\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15165" windowHeight="2445"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -380,7 +376,7 @@
   <dimension ref="B2:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,8 +431,20 @@
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
       <c r="F4">
         <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>7</v>
@@ -455,30 +463,42 @@
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5">
+        <v>-0.3</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="J5" t="e">
+      <c r="J5">
         <f>_xlfn.STDEV.P(C4:C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K5" t="e">
+        <v>0.17888543819998318</v>
+      </c>
+      <c r="K5">
         <f>_xlfn.STDEV.P(D4:D13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L5" t="e">
+        <v>0.261725046566048</v>
+      </c>
+      <c r="L5">
         <f>_xlfn.STDEV.P(G4:G13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M5" t="e">
+        <v>0</v>
+      </c>
+      <c r="M5">
         <f>_xlfn.STDEV.P(H4:H13)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
+      <c r="C6">
+        <v>-0.5</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
       <c r="F6">
         <v>3</v>
       </c>
@@ -487,6 +507,12 @@
       <c r="B7">
         <v>4</v>
       </c>
+      <c r="C7">
+        <v>-0.1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
       <c r="F7">
         <v>4</v>
       </c>
@@ -495,6 +521,12 @@
       <c r="B8">
         <v>5</v>
       </c>
+      <c r="C8">
+        <v>0.1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="F8">
         <v>5</v>
       </c>
@@ -503,6 +535,12 @@
       <c r="B9">
         <v>6</v>
       </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>-0.1</v>
+      </c>
       <c r="F9">
         <v>6</v>
       </c>
@@ -511,6 +549,12 @@
       <c r="B10">
         <v>7</v>
       </c>
+      <c r="C10">
+        <v>-0.2</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
       <c r="F10">
         <v>7</v>
       </c>
@@ -519,6 +563,12 @@
       <c r="B11">
         <v>8</v>
       </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.1</v>
+      </c>
       <c r="F11">
         <v>8</v>
       </c>
@@ -527,6 +577,12 @@
       <c r="B12">
         <v>9</v>
       </c>
+      <c r="C12">
+        <v>0.1</v>
+      </c>
+      <c r="D12">
+        <v>-0.3</v>
+      </c>
       <c r="F12">
         <v>9</v>
       </c>
@@ -534,6 +590,12 @@
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
+      </c>
+      <c r="C13">
+        <v>-0.1</v>
+      </c>
+      <c r="D13">
+        <v>-0.3</v>
       </c>
       <c r="F13">
         <v>10</v>

</xml_diff>